<commit_message>
thêm tài liệu sprint 2
a e đọc r bổ sung thêm nhé
</commit_message>
<xml_diff>
--- a/Data/sprint1.xlsx
+++ b/Data/sprint1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TranTien\Desktop\CNPM\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TranTien\Desktop\Web\CNPM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,9 +36,6 @@
     <t>Xác định lợi ích, ý nghĩa của dự án khi được triển khai</t>
   </si>
   <si>
-    <t>Khi triển khai dự án này, sẽ giúp người đọc tra cứu thông tin sách một cách dễ dàng hơn, nhà quản lý có thể dễ dàng đưa thông tin sách đến khách khàng và quản lý sách trong kho...</t>
-  </si>
-  <si>
     <t>Xác định các chức năng của sản phẩm</t>
   </si>
   <si>
@@ -170,37 +167,48 @@
     <t>nt</t>
   </si>
   <si>
-    <t>Thiết kế database</t>
-  </si>
-  <si>
-    <t>50% đăng tin</t>
-  </si>
-  <si>
-    <t>Viết tài liệu</t>
-  </si>
-  <si>
-    <t>Bổ sung chỉnh sửa database</t>
-  </si>
-  <si>
-    <t>Chỉnh sửa giao diện</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nghiên cứu tài liệu </t>
   </si>
   <si>
-    <t>80% đăng tin</t>
-  </si>
-  <si>
-    <t>Tạo chức năng trên thanh menu</t>
-  </si>
-  <si>
-    <t>làm 60% giao diện</t>
-  </si>
-  <si>
-    <t>Hoàn thiện đăng tin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tạo giao diện hoàn thiện cho các form </t>
+    <t xml:space="preserve">TÌNH TRẠNG CHUNG HIỆN NAY CỦA NHU CẦU TÌM KIẾM VIỆC LÀM 
+-Hiện tại việc tìm kiếm công việc của sinh viên đang là một nhu cầu thiết yếu.                             - Rất nhiều nhà tuyển dụng đang có nhu cầu tuyển các sinh viên vào để đào tạo và làm việc 
+LỢI ÍCH VÀ Ý NGHĨA CỦA DỰ ÁN 
+- Giúp sinh viên có được việc làm phù hợp       
+-  Sinh viên tích lũy được kinh nghiệm khi đi làm thực tế                                                               - Nhà tuyển dụng có được nhưng nhân viên đầy nhiệt huyết và thông minh
+Vậy nó đã giải quyết được những vấn đề sau :
+-  Sinh viên hiện nay chưa có việc làm phù hơp ( trái ngành ) chưa có nhiều kinh nghiệm, chưa có môi trường rèn luyện phù hợp
+- Trong quá trình học tập trên trường sinh viên chưa có kinh nghiệm nhiều trong công việc, nên sau khi học xong rất khó kiếm được việc
+</t>
+  </si>
+  <si>
+    <t>Thiết kế database, viết user story cho chức năng đăng tin</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện website</t>
+  </si>
+  <si>
+    <t>Viết userstory chức năng sửa , xóa tin</t>
+  </si>
+  <si>
+    <t>Viết userstory chức năng hiển thị tin</t>
+  </si>
+  <si>
+    <t>60% chức năng đăng tin</t>
+  </si>
+  <si>
+    <t>Hoàn thành giao diện</t>
+  </si>
+  <si>
+    <t>60% chức năng sửa tin xóa tin</t>
+  </si>
+  <si>
+    <t>60% chức năng hiện tin</t>
+  </si>
+  <si>
+    <t>tích hợp vào giao diện trang web</t>
+  </si>
+  <si>
+    <t>bug lỗi giao diện</t>
   </si>
 </sst>
 </file>
@@ -492,7 +500,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -536,6 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1119,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1132,20 +1140,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="A1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="A2" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1155,13 +1163,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1169,7 +1177,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -1178,57 +1186,57 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>3</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>39</v>
+      <c r="B6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="5" t="s">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="5" t="s">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.2">
@@ -1236,10 +1244,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="5"/>
     </row>
@@ -1248,10 +1256,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -1260,10 +1268,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -1272,10 +1280,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5"/>
     </row>
@@ -1284,10 +1292,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>27</v>
+        <v>8</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="D15" s="5"/>
     </row>
@@ -1296,10 +1304,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>40</v>
+        <v>9</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="D16" s="5"/>
     </row>
@@ -1308,13 +1316,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>30</v>
+        <v>18</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1322,10 +1330,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="9"/>
     </row>
@@ -1373,7 +1381,7 @@
   <dimension ref="E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1392,7 +1400,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1403,193 +1411,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="A1" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="15" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="29">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="30">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="29">
+        <v>2</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="29"/>
+      <c r="B9" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
+      <c r="B10" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="29">
+        <v>3</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="15" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
+      <c r="B12" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="15" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
+      <c r="B14" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="30">
-        <v>2</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="29">
+        <v>4</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="29"/>
+      <c r="B16" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="15" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="29"/>
+      <c r="B17" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="15" t="s">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="29"/>
+      <c r="B18" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="30">
-        <v>3</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="30"/>
-      <c r="B12" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
-      <c r="B13" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="30"/>
-      <c r="B14" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="30">
-        <v>4</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
-      <c r="B16" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="30" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1608,13 +1616,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="4" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>